<commit_message>
Updated and finished QA
</commit_message>
<xml_diff>
--- a/documents/s.w.a.g_-_QA_documentation.xlsx
+++ b/documents/s.w.a.g_-_QA_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITRO 5\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92D5B4C8-AFC3-4357-BFEF-8CE534022894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EC02E6F-D0F9-41E0-BACD-ABA2890AB75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1032" yWindow="1920" windowWidth="13500" windowHeight="9360" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1032" yWindow="1920" windowWidth="13500" windowHeight="9360" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map.cpp" sheetId="6" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="Serbia.cpp" sheetId="13" r:id="rId8"/>
     <sheet name="Romania.cpp" sheetId="14" r:id="rId9"/>
     <sheet name="Turkey.cpp" sheetId="15" r:id="rId10"/>
+    <sheet name="map.cpp 0.1" sheetId="16" r:id="rId11"/>
+    <sheet name="functions.cpp 0.1" sheetId="17" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="126">
   <si>
     <t>TEST CASE 1</t>
   </si>
@@ -923,6 +925,208 @@
   </si>
   <si>
     <t>TR_LOADS</t>
+  </si>
+  <si>
+    <t>TEST CASE 17</t>
+  </si>
+  <si>
+    <t>Displays a screen with a message when the game is finished</t>
+  </si>
+  <si>
+    <r>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> drawEndScreen()</t>
+    </r>
+  </si>
+  <si>
+    <t>When you finish the game it shows you a message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The functions shows you the expected message </t>
+  </si>
+  <si>
+    <t>ESC_DISPLAYS</t>
+  </si>
+  <si>
+    <t>TEST CASE 18</t>
+  </si>
+  <si>
+    <t>Displays a message when the chosen country is not finished yet</t>
+  </si>
+  <si>
+    <r>
+      <t>void</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> drawComingSoonPrompt(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF2B91AF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Texture2D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>background</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>promptChoice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF2B91AF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Color</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>color</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>bool</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>isBulgaria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>When you press the country and it's not finished it gives you a message</t>
+  </si>
+  <si>
+    <t>The function shows you the expected message.</t>
+  </si>
+  <si>
+    <t>CMS_DISPLAYS</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1850,7 @@
   <dimension ref="B1:I51"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1782,12 +1986,12 @@
     <row r="10" spans="2:9" ht="15"/>
     <row r="11" spans="2:9" ht="14.45" customHeight="1"/>
     <row r="12" spans="2:9" ht="14.45" customHeight="1"/>
-    <row r="13" spans="2:9" ht="15" customHeight="1"/>
-    <row r="14" spans="2:9" ht="15" customHeight="1"/>
+    <row r="13" spans="2:9" ht="15"/>
+    <row r="14" spans="2:9" ht="15"/>
     <row r="15" spans="2:9" ht="14.45" customHeight="1"/>
     <row r="16" spans="2:9" ht="14.45" customHeight="1"/>
     <row r="17" ht="15"/>
-    <row r="18" ht="15" customHeight="1"/>
+    <row r="18" ht="15"/>
     <row r="19" ht="15"/>
     <row r="20" ht="15"/>
     <row r="21" ht="15"/>
@@ -1839,7 +2043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4BDB49B-C994-49ED-8709-7F8D4BAE5473}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -1952,6 +2156,296 @@
       <c r="H7" s="40"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" customHeight="1">
+      <c r="A8" s="24"/>
+      <c r="B8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="H6:H8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298A0009-CB19-496D-9311-B8AE6DD7B0C8}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.45" customHeight="1"/>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" customHeight="1">
+      <c r="A6" s="22">
+        <v>17</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1">
+      <c r="A7" s="23"/>
+      <c r="B7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="40"/>
+    </row>
+    <row r="8" spans="1:8" ht="42.75" customHeight="1">
+      <c r="A8" s="24"/>
+      <c r="B8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="H6:H8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFDCFA5-B35E-479A-827D-0217DB7D9E46}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.45" customHeight="1"/>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" customHeight="1">
+      <c r="A6" s="22">
+        <v>17</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1">
+      <c r="A7" s="23"/>
+      <c r="B7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="40"/>
+    </row>
+    <row r="8" spans="1:8" ht="96.75" customHeight="1">
       <c r="A8" s="24"/>
       <c r="B8" s="13" t="s">
         <v>17</v>
@@ -2562,6 +3056,22 @@
     <row r="48" ht="15"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B1:I2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="B13:I14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="F18:F20"/>
     <mergeCell ref="B25:I26"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="B30:B32"/>
@@ -2570,22 +3080,6 @@
     <mergeCell ref="H30:H32"/>
     <mergeCell ref="I30:I32"/>
     <mergeCell ref="F30:F32"/>
-    <mergeCell ref="B13:I14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="B1:I2"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="F6:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3196,6 +3690,38 @@
     <row r="53" spans="2:9" ht="15"/>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B1:I2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="B13:I14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="B24:I25"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="B36:I37"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="I41:I43"/>
     <mergeCell ref="B45:I46"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="B50:B52"/>
@@ -3204,38 +3730,6 @@
     <mergeCell ref="G50:G52"/>
     <mergeCell ref="H50:H52"/>
     <mergeCell ref="I50:I52"/>
-    <mergeCell ref="B36:I37"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="I41:I43"/>
-    <mergeCell ref="B24:I25"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="B13:I14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="B1:I2"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="F6:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FInished featured update on QA
</commit_message>
<xml_diff>
--- a/documents/s.w.a.g_-_QA_documentation.xlsx
+++ b/documents/s.w.a.g_-_QA_documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITRO 5\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EC02E6F-D0F9-41E0-BACD-ABA2890AB75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9ECDABE-9FCC-4D13-AFEC-9DCF1B49601A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1032" yWindow="1920" windowWidth="13500" windowHeight="9360" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1032" yWindow="1920" windowWidth="13500" windowHeight="9360" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map.cpp" sheetId="6" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Turkey.cpp" sheetId="15" r:id="rId10"/>
     <sheet name="map.cpp 0.1" sheetId="16" r:id="rId11"/>
     <sheet name="functions.cpp 0.1" sheetId="17" r:id="rId12"/>
+    <sheet name="bulgaria.cpp 0.1" sheetId="18" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="132">
   <si>
     <t>TEST CASE 1</t>
   </si>
@@ -1127,6 +1128,251 @@
   </si>
   <si>
     <t>CMS_DISPLAYS</t>
+  </si>
+  <si>
+    <t>TEST CASE 19</t>
+  </si>
+  <si>
+    <t>Displays the tutorial text</t>
+  </si>
+  <si>
+    <r>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> drawMentorText(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF2B91AF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Texture2D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>background</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF2B91AF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Texture2D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>mentor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>char</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>message</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[], </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>char</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>newLines</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[], </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <charset val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>When you press on Bulgaria it shows the tutorial</t>
+  </si>
+  <si>
+    <t>The function shows you how to play the game</t>
+  </si>
+  <si>
+    <t>TXT_DISPLAY</t>
   </si>
 </sst>
 </file>
@@ -2333,7 +2579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFDCFA5-B35E-479A-827D-0217DB7D9E46}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -2446,6 +2692,151 @@
       <c r="H7" s="40"/>
     </row>
     <row r="8" spans="1:8" ht="96.75" customHeight="1">
+      <c r="A8" s="24"/>
+      <c r="B8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="H6:H8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6D192C-BC2B-4AF7-A192-6F5DCBAADBF1}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.45" customHeight="1"/>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" customHeight="1">
+      <c r="A6" s="22">
+        <v>17</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1">
+      <c r="A7" s="23"/>
+      <c r="B7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="40"/>
+    </row>
+    <row r="8" spans="1:8" ht="82.5" customHeight="1">
       <c r="A8" s="24"/>
       <c r="B8" s="13" t="s">
         <v>17</v>
@@ -3056,6 +3447,22 @@
     <row r="48" ht="15"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B25:I26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="H30:H32"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="B13:I14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="F18:F20"/>
     <mergeCell ref="B1:I2"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="B6:B8"/>
@@ -3064,22 +3471,6 @@
     <mergeCell ref="H6:H8"/>
     <mergeCell ref="I6:I8"/>
     <mergeCell ref="F6:F8"/>
-    <mergeCell ref="B13:I14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="B25:I26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="G30:G32"/>
-    <mergeCell ref="H30:H32"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="F30:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3690,6 +4081,38 @@
     <row r="53" spans="2:9" ht="15"/>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B45:I46"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="I50:I52"/>
+    <mergeCell ref="B36:I37"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="I41:I43"/>
+    <mergeCell ref="B24:I25"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="B13:I14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="F18:F20"/>
     <mergeCell ref="B1:I2"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="B6:B8"/>
@@ -3698,38 +4121,6 @@
     <mergeCell ref="H6:H8"/>
     <mergeCell ref="I6:I8"/>
     <mergeCell ref="F6:F8"/>
-    <mergeCell ref="B13:I14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="B24:I25"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="B36:I37"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="I41:I43"/>
-    <mergeCell ref="B45:I46"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="H50:H52"/>
-    <mergeCell ref="I50:I52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>